<commit_message>
Bỏ chữ NAM THUẬN
</commit_message>
<xml_diff>
--- a/static/uploads/mau/bangcong/mau_bangchamcong_hanhchinh.xlsx
+++ b/static/uploads/mau/bangcong/mau_bangchamcong_hanhchinh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAT\Desktop\code\working\HRM\static\uploads\mau\bangcong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2803F9-55B9-4429-A83F-8BD868F9BE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D98F7D-5518-4AE5-9BDA-33D58565A28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0B459C31-F691-4EE8-A3E0-D773EEF2E69F}"/>
   </bookViews>
@@ -30,9 +30,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
-    <t>BẢNG CHẤM CÔNG HÀNH CHÍNH NAM THUẬN</t>
-  </si>
-  <si>
     <t>THÁNG 10 NĂM 2024</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>Chính thức</t>
+  </si>
+  <si>
+    <t>BẢNG CHẤM CÔNG HÀNH CHÍNH</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
       <pane xSplit="9" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ4" sqref="AQ1:AS1048576"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:AP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
   <sheetData>
     <row r="1" spans="1:42" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -653,7 +653,7 @@
     </row>
     <row r="2" spans="1:42" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -743,130 +743,130 @@
     </row>
     <row r="4" spans="1:42" s="2" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AJ4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AJ4" s="1" t="s">
+      <c r="AK4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AL4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AM4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AO4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>